<commit_message>
include formula in csv export
</commit_message>
<xml_diff>
--- a/src/Tests/sample.xlsx
+++ b/src/Tests/sample.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\VerifyTests\Verify.Aspose\src\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Verify.Aspose\src\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAB36F4-5C13-4639-A094-1D32A9DD0150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2010209-0056-43E3-802F-A9A8640FC6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="4980" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="30">
   <si>
     <t>First Name</t>
   </si>
@@ -107,6 +118,9 @@
   </si>
   <si>
     <t>Weiland</t>
+  </si>
+  <si>
+    <t>Formula</t>
   </si>
 </sst>
 </file>
@@ -123,10 +137,12 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,9 +166,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -501,7 +517,9 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -542,6 +560,10 @@
       <c r="G2">
         <v>1562</v>
       </c>
+      <c r="H2">
+        <f>G2+A2</f>
+        <v>1563</v>
+      </c>
     </row>
     <row r="3" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -565,6 +587,10 @@
       <c r="G3">
         <v>1582</v>
       </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H46" si="0">G3+A3</f>
+        <v>1584</v>
+      </c>
     </row>
     <row r="4" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -588,6 +614,10 @@
       <c r="G4">
         <v>2587</v>
       </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>2590</v>
+      </c>
     </row>
     <row r="5" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -611,6 +641,10 @@
       <c r="G5">
         <v>3549</v>
       </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>3553</v>
+      </c>
     </row>
     <row r="6" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -634,6 +668,10 @@
       <c r="G6">
         <v>2468</v>
       </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>2473</v>
+      </c>
     </row>
     <row r="7" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -657,6 +695,10 @@
       <c r="G7">
         <v>2554</v>
       </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>2560</v>
+      </c>
     </row>
     <row r="8" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -680,6 +722,10 @@
       <c r="G8">
         <v>3598</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>3605</v>
+      </c>
     </row>
     <row r="9" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -703,6 +749,10 @@
       <c r="G9">
         <v>2456</v>
       </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>2464</v>
+      </c>
     </row>
     <row r="10" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -725,6 +775,10 @@
       </c>
       <c r="G10">
         <v>6548</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>6557</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -749,6 +803,10 @@
       <c r="G11">
         <v>1562</v>
       </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>1563</v>
+      </c>
     </row>
     <row r="12" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -772,6 +830,10 @@
       <c r="G12">
         <v>1582</v>
       </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>1584</v>
+      </c>
     </row>
     <row r="13" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -795,6 +857,10 @@
       <c r="G13">
         <v>2587</v>
       </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>2590</v>
+      </c>
     </row>
     <row r="14" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -818,6 +884,10 @@
       <c r="G14">
         <v>3549</v>
       </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>3553</v>
+      </c>
     </row>
     <row r="15" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -841,6 +911,10 @@
       <c r="G15">
         <v>2468</v>
       </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>2473</v>
+      </c>
     </row>
     <row r="16" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -864,8 +938,12 @@
       <c r="G16">
         <v>2554</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>7</v>
       </c>
@@ -887,8 +965,12 @@
       <c r="G17">
         <v>3598</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>3605</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>8</v>
       </c>
@@ -910,8 +992,12 @@
       <c r="G18">
         <v>2456</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>2464</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>9</v>
       </c>
@@ -933,8 +1019,12 @@
       <c r="G19">
         <v>6548</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>6557</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -956,8 +1046,12 @@
       <c r="G20">
         <v>1562</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -979,8 +1073,12 @@
       <c r="G21">
         <v>1582</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1002,8 +1100,12 @@
       <c r="G22">
         <v>2587</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1025,8 +1127,12 @@
       <c r="G23">
         <v>3549</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>3553</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5</v>
       </c>
@@ -1048,8 +1154,12 @@
       <c r="G24">
         <v>2468</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>2473</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1071,8 +1181,12 @@
       <c r="G25">
         <v>2554</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>7</v>
       </c>
@@ -1094,8 +1208,12 @@
       <c r="G26">
         <v>3598</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>3605</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>8</v>
       </c>
@@ -1117,8 +1235,12 @@
       <c r="G27">
         <v>2456</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>2464</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1140,8 +1262,12 @@
       <c r="G28">
         <v>6548</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>6557</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1163,8 +1289,12 @@
       <c r="G29">
         <v>1562</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1186,8 +1316,12 @@
       <c r="G30">
         <v>1582</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1209,8 +1343,12 @@
       <c r="G31">
         <v>2587</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -1232,8 +1370,12 @@
       <c r="G32">
         <v>3549</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>3553</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>5</v>
       </c>
@@ -1255,8 +1397,12 @@
       <c r="G33">
         <v>2468</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>2473</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>6</v>
       </c>
@@ -1278,8 +1424,12 @@
       <c r="G34">
         <v>2554</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>7</v>
       </c>
@@ -1301,8 +1451,12 @@
       <c r="G35">
         <v>3598</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>3605</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>8</v>
       </c>
@@ -1324,8 +1478,12 @@
       <c r="G36">
         <v>2456</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>2464</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>9</v>
       </c>
@@ -1347,8 +1505,12 @@
       <c r="G37">
         <v>6548</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>6557</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1370,8 +1532,12 @@
       <c r="G38">
         <v>1562</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1393,8 +1559,12 @@
       <c r="G39">
         <v>1582</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3</v>
       </c>
@@ -1416,8 +1586,12 @@
       <c r="G40">
         <v>2587</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1439,8 +1613,12 @@
       <c r="G41">
         <v>3549</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>3553</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>5</v>
       </c>
@@ -1462,8 +1640,12 @@
       <c r="G42">
         <v>2468</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>2473</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>6</v>
       </c>
@@ -1485,8 +1667,12 @@
       <c r="G43">
         <v>2554</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>7</v>
       </c>
@@ -1508,8 +1694,12 @@
       <c r="G44">
         <v>3598</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>3605</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>8</v>
       </c>
@@ -1531,8 +1721,12 @@
       <c r="G45">
         <v>2456</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H45">
+        <f t="shared" si="0"/>
+        <v>2464</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>9</v>
       </c>
@@ -1554,9 +1748,13 @@
       <c r="G46">
         <v>6548</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="H46">
+        <f t="shared" si="0"/>
+        <v>6557</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>